<commit_message>
added report and data sheets
</commit_message>
<xml_diff>
--- a/cpp/dynamic_programming/data.xlsx
+++ b/cpp/dynamic_programming/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="MCSS" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="15">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -249,7 +249,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart145.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -527,11 +527,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="77994001"/>
-        <c:axId val="63214744"/>
+        <c:axId val="697774"/>
+        <c:axId val="27769832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77994001"/>
+        <c:axId val="697774"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63214744"/>
+        <c:crossAx val="27769832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -571,7 +571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63214744"/>
+        <c:axId val="27769832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +610,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77994001"/>
+        <c:crossAx val="697774"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -662,7 +662,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart146.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -958,11 +958,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="33986817"/>
-        <c:axId val="43893809"/>
+        <c:axId val="93392343"/>
+        <c:axId val="82366275"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="33986817"/>
+        <c:axId val="93392343"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,7 +994,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43893809"/>
+        <c:crossAx val="82366275"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1002,7 +1002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43893809"/>
+        <c:axId val="82366275"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1041,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33986817"/>
+        <c:crossAx val="93392343"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1093,7 +1093,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart147.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1389,11 +1389,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="25607876"/>
-        <c:axId val="18693544"/>
+        <c:axId val="137294"/>
+        <c:axId val="74881133"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25607876"/>
+        <c:axId val="137294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1425,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18693544"/>
+        <c:crossAx val="74881133"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1433,7 +1433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18693544"/>
+        <c:axId val="74881133"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,7 +1472,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25607876"/>
+        <c:crossAx val="137294"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1524,7 +1524,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart148.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1820,11 +1820,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="70211379"/>
-        <c:axId val="7874238"/>
+        <c:axId val="96312184"/>
+        <c:axId val="816616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70211379"/>
+        <c:axId val="96312184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1856,7 +1856,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7874238"/>
+        <c:crossAx val="816616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1864,7 +1864,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7874238"/>
+        <c:axId val="816616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,7 +1903,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70211379"/>
+        <c:crossAx val="96312184"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1955,7 +1955,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart149.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2257,11 +2257,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="1582935"/>
-        <c:axId val="660012"/>
+        <c:axId val="77932839"/>
+        <c:axId val="56764338"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1582935"/>
+        <c:axId val="77932839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2293,7 +2293,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="660012"/>
+        <c:crossAx val="56764338"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2301,7 +2301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="660012"/>
+        <c:axId val="56764338"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2340,7 +2340,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1582935"/>
+        <c:crossAx val="77932839"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2392,7 +2392,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart150.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2694,11 +2694,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="20653268"/>
-        <c:axId val="10391920"/>
+        <c:axId val="20370628"/>
+        <c:axId val="85398741"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="20653268"/>
+        <c:axId val="20370628"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2730,7 +2730,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10391920"/>
+        <c:crossAx val="85398741"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2738,7 +2738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10391920"/>
+        <c:axId val="85398741"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2777,7 +2777,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20653268"/>
+        <c:crossAx val="20370628"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2829,7 +2829,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart151.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3131,11 +3131,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="30123104"/>
-        <c:axId val="18615069"/>
+        <c:axId val="21080876"/>
+        <c:axId val="32834432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30123104"/>
+        <c:axId val="21080876"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3167,7 +3167,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18615069"/>
+        <c:crossAx val="32834432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3175,7 +3175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18615069"/>
+        <c:axId val="32834432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3214,7 +3214,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30123104"/>
+        <c:crossAx val="21080876"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3266,7 +3266,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart152.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3568,11 +3568,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="47129566"/>
-        <c:axId val="7286082"/>
+        <c:axId val="86766217"/>
+        <c:axId val="16351533"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47129566"/>
+        <c:axId val="86766217"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3604,7 +3604,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7286082"/>
+        <c:crossAx val="16351533"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3612,7 +3612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7286082"/>
+        <c:axId val="16351533"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3651,7 +3651,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47129566"/>
+        <c:crossAx val="86766217"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3703,7 +3703,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart153.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4008,11 +4008,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="84127408"/>
-        <c:axId val="85747536"/>
+        <c:axId val="7533081"/>
+        <c:axId val="67587258"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84127408"/>
+        <c:axId val="7533081"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4044,7 +4044,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85747536"/>
+        <c:crossAx val="67587258"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4052,7 +4052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85747536"/>
+        <c:axId val="67587258"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4091,7 +4091,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84127408"/>
+        <c:crossAx val="7533081"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4143,7 +4143,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart154.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4445,11 +4445,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="94314027"/>
-        <c:axId val="30148096"/>
+        <c:axId val="40864253"/>
+        <c:axId val="68811098"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94314027"/>
+        <c:axId val="40864253"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4481,7 +4481,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30148096"/>
+        <c:crossAx val="68811098"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4489,7 +4489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30148096"/>
+        <c:axId val="68811098"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4528,7 +4528,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94314027"/>
+        <c:crossAx val="40864253"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4580,7 +4580,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart155.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4882,11 +4882,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="84202411"/>
-        <c:axId val="9915477"/>
+        <c:axId val="31243244"/>
+        <c:axId val="66312997"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84202411"/>
+        <c:axId val="31243244"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4918,7 +4918,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9915477"/>
+        <c:crossAx val="66312997"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4926,7 +4926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9915477"/>
+        <c:axId val="66312997"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4965,7 +4965,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84202411"/>
+        <c:crossAx val="31243244"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5017,7 +5017,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart156.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5319,11 +5319,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="40591751"/>
-        <c:axId val="22390158"/>
+        <c:axId val="54731530"/>
+        <c:axId val="29306138"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40591751"/>
+        <c:axId val="54731530"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5355,7 +5355,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22390158"/>
+        <c:crossAx val="29306138"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5363,7 +5363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22390158"/>
+        <c:axId val="29306138"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5402,7 +5402,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40591751"/>
+        <c:crossAx val="54731530"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5454,7 +5454,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart157.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5750,11 +5750,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="19802686"/>
-        <c:axId val="80175037"/>
+        <c:axId val="75672441"/>
+        <c:axId val="14676219"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="19802686"/>
+        <c:axId val="75672441"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5786,7 +5786,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80175037"/>
+        <c:crossAx val="14676219"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5794,7 +5794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80175037"/>
+        <c:axId val="14676219"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5833,7 +5833,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19802686"/>
+        <c:crossAx val="75672441"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5885,7 +5885,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart158.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6181,11 +6181,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="91912138"/>
-        <c:axId val="86954099"/>
+        <c:axId val="75408644"/>
+        <c:axId val="46065539"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91912138"/>
+        <c:axId val="75408644"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6217,7 +6217,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86954099"/>
+        <c:crossAx val="46065539"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6225,7 +6225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86954099"/>
+        <c:axId val="46065539"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6264,7 +6264,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91912138"/>
+        <c:crossAx val="75408644"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6316,7 +6316,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart159.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6612,11 +6612,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="23836050"/>
-        <c:axId val="54947108"/>
+        <c:axId val="12403462"/>
+        <c:axId val="20773676"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="23836050"/>
+        <c:axId val="12403462"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6648,7 +6648,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54947108"/>
+        <c:crossAx val="20773676"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6656,7 +6656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54947108"/>
+        <c:axId val="20773676"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6695,7 +6695,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23836050"/>
+        <c:crossAx val="12403462"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6747,7 +6747,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart160.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7043,11 +7043,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="69929539"/>
-        <c:axId val="45764431"/>
+        <c:axId val="1461091"/>
+        <c:axId val="84435546"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69929539"/>
+        <c:axId val="1461091"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7079,7 +7079,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45764431"/>
+        <c:crossAx val="84435546"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7087,7 +7087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45764431"/>
+        <c:axId val="84435546"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7126,7 +7126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69929539"/>
+        <c:crossAx val="1461091"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7178,7 +7178,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart161.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7462,11 +7462,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="74566269"/>
-        <c:axId val="94815587"/>
+        <c:axId val="80721822"/>
+        <c:axId val="7699033"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74566269"/>
+        <c:axId val="80721822"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7498,7 +7498,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94815587"/>
+        <c:crossAx val="7699033"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7506,7 +7506,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94815587"/>
+        <c:axId val="7699033"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7545,7 +7545,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74566269"/>
+        <c:crossAx val="80721822"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7597,7 +7597,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart162.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7881,11 +7881,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="78759162"/>
-        <c:axId val="35650566"/>
+        <c:axId val="87682794"/>
+        <c:axId val="81551164"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78759162"/>
+        <c:axId val="87682794"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7917,7 +7917,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35650566"/>
+        <c:crossAx val="81551164"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7925,7 +7925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35650566"/>
+        <c:axId val="81551164"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7964,7 +7964,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78759162"/>
+        <c:crossAx val="87682794"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8016,7 +8016,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart163.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8300,11 +8300,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="15194704"/>
-        <c:axId val="21972212"/>
+        <c:axId val="52829739"/>
+        <c:axId val="54589911"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15194704"/>
+        <c:axId val="52829739"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8336,7 +8336,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21972212"/>
+        <c:crossAx val="54589911"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8344,7 +8344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="21972212"/>
+        <c:axId val="54589911"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8383,7 +8383,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15194704"/>
+        <c:crossAx val="52829739"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8435,7 +8435,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart164.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8719,11 +8719,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="28712250"/>
-        <c:axId val="26471968"/>
+        <c:axId val="42077548"/>
+        <c:axId val="65455000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28712250"/>
+        <c:axId val="42077548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8755,7 +8755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26471968"/>
+        <c:crossAx val="65455000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8763,7 +8763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26471968"/>
+        <c:axId val="65455000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8802,7 +8802,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28712250"/>
+        <c:crossAx val="42077548"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8854,7 +8854,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart165.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9150,11 +9150,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="49998328"/>
-        <c:axId val="59742794"/>
+        <c:axId val="61382333"/>
+        <c:axId val="70248901"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49998328"/>
+        <c:axId val="61382333"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9186,7 +9186,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59742794"/>
+        <c:crossAx val="70248901"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9194,7 +9194,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59742794"/>
+        <c:axId val="70248901"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9233,7 +9233,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49998328"/>
+        <c:crossAx val="61382333"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9285,7 +9285,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart166.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9581,11 +9581,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="88257099"/>
-        <c:axId val="79600996"/>
+        <c:axId val="91919246"/>
+        <c:axId val="58088295"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88257099"/>
+        <c:axId val="91919246"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9617,7 +9617,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79600996"/>
+        <c:crossAx val="58088295"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9625,7 +9625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79600996"/>
+        <c:axId val="58088295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9664,7 +9664,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88257099"/>
+        <c:crossAx val="91919246"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9716,7 +9716,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart167.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -10012,11 +10012,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="8005695"/>
-        <c:axId val="26737787"/>
+        <c:axId val="73974357"/>
+        <c:axId val="22982959"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8005695"/>
+        <c:axId val="73974357"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10048,7 +10048,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26737787"/>
+        <c:crossAx val="22982959"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10056,7 +10056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26737787"/>
+        <c:axId val="22982959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10095,7 +10095,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8005695"/>
+        <c:crossAx val="73974357"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10147,7 +10147,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart168.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -10443,11 +10443,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="94447183"/>
-        <c:axId val="72312061"/>
+        <c:axId val="94187930"/>
+        <c:axId val="45039044"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94447183"/>
+        <c:axId val="94187930"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10479,7 +10479,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72312061"/>
+        <c:crossAx val="45039044"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10487,7 +10487,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72312061"/>
+        <c:axId val="45039044"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10526,7 +10526,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94447183"/>
+        <c:crossAx val="94187930"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10578,7 +10578,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart169.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -10874,11 +10874,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="56465333"/>
-        <c:axId val="55953360"/>
+        <c:axId val="30780491"/>
+        <c:axId val="65296698"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56465333"/>
+        <c:axId val="30780491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10910,7 +10910,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55953360"/>
+        <c:crossAx val="65296698"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10918,7 +10918,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55953360"/>
+        <c:axId val="65296698"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10957,7 +10957,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56465333"/>
+        <c:crossAx val="30780491"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11009,7 +11009,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart170.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -11305,11 +11305,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="2646674"/>
-        <c:axId val="93009401"/>
+        <c:axId val="43676001"/>
+        <c:axId val="91576849"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2646674"/>
+        <c:axId val="43676001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11341,7 +11341,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93009401"/>
+        <c:crossAx val="91576849"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11349,7 +11349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93009401"/>
+        <c:axId val="91576849"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11388,7 +11388,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2646674"/>
+        <c:crossAx val="43676001"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11440,7 +11440,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart171.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -11736,11 +11736,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="8945896"/>
-        <c:axId val="75215823"/>
+        <c:axId val="78913663"/>
+        <c:axId val="34113020"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8945896"/>
+        <c:axId val="78913663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11772,7 +11772,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75215823"/>
+        <c:crossAx val="34113020"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11780,7 +11780,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75215823"/>
+        <c:axId val="34113020"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11819,7 +11819,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8945896"/>
+        <c:crossAx val="78913663"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11871,7 +11871,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart172.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart64.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -12143,11 +12143,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="89993126"/>
-        <c:axId val="70010403"/>
+        <c:axId val="48865576"/>
+        <c:axId val="74936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89993126"/>
+        <c:axId val="48865576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12179,7 +12179,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70010403"/>
+        <c:crossAx val="74936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12187,7 +12187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70010403"/>
+        <c:axId val="74936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12226,7 +12226,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89993126"/>
+        <c:crossAx val="48865576"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12278,7 +12278,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart173.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart65.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -12559,11 +12559,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="55809196"/>
-        <c:axId val="47944534"/>
+        <c:axId val="61867034"/>
+        <c:axId val="1739047"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55809196"/>
+        <c:axId val="61867034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12595,7 +12595,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47944534"/>
+        <c:crossAx val="1739047"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12603,7 +12603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47944534"/>
+        <c:axId val="1739047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12642,7 +12642,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55809196"/>
+        <c:crossAx val="61867034"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12694,7 +12694,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart174.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart66.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -12984,11 +12984,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="4157849"/>
-        <c:axId val="9368372"/>
+        <c:axId val="52978205"/>
+        <c:axId val="87532101"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="4157849"/>
+        <c:axId val="52978205"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13020,7 +13020,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9368372"/>
+        <c:crossAx val="87532101"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13028,7 +13028,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9368372"/>
+        <c:axId val="87532101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13067,7 +13067,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4157849"/>
+        <c:crossAx val="52978205"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13119,7 +13119,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart175.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart67.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -13409,11 +13409,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="25158389"/>
-        <c:axId val="88985326"/>
+        <c:axId val="16755516"/>
+        <c:axId val="32878401"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25158389"/>
+        <c:axId val="16755516"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13445,7 +13445,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88985326"/>
+        <c:crossAx val="32878401"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13453,7 +13453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88985326"/>
+        <c:axId val="32878401"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13492,7 +13492,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25158389"/>
+        <c:crossAx val="16755516"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13544,7 +13544,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart176.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -13810,11 +13810,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="15938499"/>
-        <c:axId val="28721499"/>
+        <c:axId val="56600595"/>
+        <c:axId val="16902150"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15938499"/>
+        <c:axId val="56600595"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13846,7 +13846,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28721499"/>
+        <c:crossAx val="16902150"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13854,7 +13854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28721499"/>
+        <c:axId val="16902150"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13893,7 +13893,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15938499"/>
+        <c:crossAx val="56600595"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13945,7 +13945,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart177.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart69.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -14229,11 +14229,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="61482108"/>
-        <c:axId val="99578336"/>
+        <c:axId val="60944760"/>
+        <c:axId val="18932349"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61482108"/>
+        <c:axId val="60944760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14265,7 +14265,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99578336"/>
+        <c:crossAx val="18932349"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14273,7 +14273,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99578336"/>
+        <c:axId val="18932349"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14312,7 +14312,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61482108"/>
+        <c:crossAx val="60944760"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14364,7 +14364,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart178.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart70.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -14654,11 +14654,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="75225879"/>
-        <c:axId val="8282958"/>
+        <c:axId val="45112552"/>
+        <c:axId val="26808140"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75225879"/>
+        <c:axId val="45112552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14690,7 +14690,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8282958"/>
+        <c:crossAx val="26808140"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14698,7 +14698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8282958"/>
+        <c:axId val="26808140"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14737,7 +14737,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75225879"/>
+        <c:crossAx val="45112552"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14789,7 +14789,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart179.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart71.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15079,11 +15079,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="22342808"/>
-        <c:axId val="51311949"/>
+        <c:axId val="33646735"/>
+        <c:axId val="90227779"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22342808"/>
+        <c:axId val="33646735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15115,7 +15115,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51311949"/>
+        <c:crossAx val="90227779"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15123,7 +15123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51311949"/>
+        <c:axId val="90227779"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15162,7 +15162,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22342808"/>
+        <c:crossAx val="33646735"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15214,7 +15214,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart180.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart72.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -15480,11 +15480,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="50663174"/>
-        <c:axId val="67900669"/>
+        <c:axId val="77222984"/>
+        <c:axId val="96819458"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50663174"/>
+        <c:axId val="77222984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15516,7 +15516,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67900669"/>
+        <c:crossAx val="96819458"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15524,7 +15524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67900669"/>
+        <c:axId val="96819458"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15563,7 +15563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50663174"/>
+        <c:crossAx val="77222984"/>
         <c:crosses val="min"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15626,9 +15626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
+      <xdr:colOff>675720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15637,7 +15637,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16940880" y="374760"/>
-        <a:ext cx="4933800" cy="2782800"/>
+        <a:ext cx="4933440" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15656,9 +15656,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>586800</xdr:colOff>
+      <xdr:colOff>586440</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15667,7 +15667,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16853760" y="3498480"/>
-        <a:ext cx="4931640" cy="2782800"/>
+        <a:ext cx="4931280" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15686,9 +15686,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>566280</xdr:colOff>
+      <xdr:colOff>565920</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15697,7 +15697,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16833240" y="6309360"/>
-        <a:ext cx="4931640" cy="2780280"/>
+        <a:ext cx="4931280" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15716,9 +15716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>500400</xdr:colOff>
+      <xdr:colOff>500040</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15727,7 +15727,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16767360" y="9113400"/>
-        <a:ext cx="4931640" cy="2780280"/>
+        <a:ext cx="4931280" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15751,9 +15751,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
+      <xdr:colOff>675720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15762,7 +15762,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16940880" y="374760"/>
-        <a:ext cx="4933800" cy="2782800"/>
+        <a:ext cx="4933440" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15781,9 +15781,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>586800</xdr:colOff>
+      <xdr:colOff>586440</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15792,7 +15792,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16853760" y="3498480"/>
-        <a:ext cx="4931640" cy="2782800"/>
+        <a:ext cx="4931280" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15811,9 +15811,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>566280</xdr:colOff>
+      <xdr:colOff>565920</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15822,7 +15822,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16833240" y="6837840"/>
-        <a:ext cx="4931640" cy="2780280"/>
+        <a:ext cx="4931280" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15841,9 +15841,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>500400</xdr:colOff>
+      <xdr:colOff>500040</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15852,7 +15852,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16767360" y="9641880"/>
-        <a:ext cx="4931640" cy="2780280"/>
+        <a:ext cx="4931280" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15869,16 +15869,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>634320</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>686520</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>676080</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>727920</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15886,8 +15886,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16940880" y="374760"/>
-        <a:ext cx="4933800" cy="2782800"/>
+        <a:off x="18623880" y="199440"/>
+        <a:ext cx="4933440" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15899,16 +15899,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>547200</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>639000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>586800</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15916,8 +15916,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16853760" y="3498480"/>
-        <a:ext cx="4931640" cy="2782800"/>
+        <a:off x="18576360" y="3525480"/>
+        <a:ext cx="4931280" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15936,9 +15936,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>566280</xdr:colOff>
+      <xdr:colOff>565920</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15947,7 +15947,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16833240" y="6837840"/>
-        <a:ext cx="4931640" cy="2780280"/>
+        <a:ext cx="4931280" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -15966,9 +15966,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>500400</xdr:colOff>
+      <xdr:colOff>500040</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -15977,7 +15977,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16767360" y="9641880"/>
-        <a:ext cx="4931640" cy="2780280"/>
+        <a:ext cx="4931280" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16001,9 +16001,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>477360</xdr:colOff>
+      <xdr:colOff>477000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16012,7 +16012,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15613920" y="374760"/>
-        <a:ext cx="4560840" cy="2782800"/>
+        <a:ext cx="4560480" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16031,9 +16031,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>394920</xdr:colOff>
+      <xdr:colOff>394560</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16042,7 +16042,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15533280" y="3498480"/>
-        <a:ext cx="4559040" cy="2782800"/>
+        <a:ext cx="4558680" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16061,9 +16061,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>375840</xdr:colOff>
+      <xdr:colOff>375480</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16072,7 +16072,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15514200" y="6309360"/>
-        <a:ext cx="4559040" cy="2780280"/>
+        <a:ext cx="4558680" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16091,9 +16091,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>315000</xdr:colOff>
+      <xdr:colOff>314640</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16102,7 +16102,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15453360" y="9113400"/>
-        <a:ext cx="4559040" cy="2780280"/>
+        <a:ext cx="4558680" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16126,9 +16126,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>27360</xdr:colOff>
+      <xdr:colOff>27000</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16137,7 +16137,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16269120" y="180000"/>
-        <a:ext cx="4560840" cy="2782800"/>
+        <a:ext cx="4560480" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16156,9 +16156,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>615600</xdr:colOff>
+      <xdr:colOff>615240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16167,7 +16167,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16188480" y="4045680"/>
-        <a:ext cx="4559040" cy="2782800"/>
+        <a:ext cx="4558680" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16186,9 +16186,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>596520</xdr:colOff>
+      <xdr:colOff>596160</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>45360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16197,7 +16197,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16169400" y="6904440"/>
-        <a:ext cx="4559040" cy="2780280"/>
+        <a:ext cx="4558680" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16216,9 +16216,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>535680</xdr:colOff>
+      <xdr:colOff>535320</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16227,7 +16227,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16108560" y="9751680"/>
-        <a:ext cx="4559040" cy="2780280"/>
+        <a:ext cx="4558680" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16244,16 +16244,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>165600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>336240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>32400</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>203040</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16261,8 +16261,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15839640" y="180000"/>
-        <a:ext cx="4560840" cy="2782800"/>
+        <a:off x="17351640" y="44640"/>
+        <a:ext cx="4560480" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16274,16 +16274,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>360720</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>620640</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>225720</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16291,8 +16291,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15759000" y="3346920"/>
-        <a:ext cx="4559040" cy="2782800"/>
+        <a:off x="17376120" y="3360600"/>
+        <a:ext cx="4558680" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16311,9 +16311,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>601560</xdr:colOff>
+      <xdr:colOff>601200</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>43200</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16322,7 +16322,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15739920" y="6201000"/>
-        <a:ext cx="4559040" cy="2780280"/>
+        <a:ext cx="4558680" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16341,9 +16341,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>540720</xdr:colOff>
+      <xdr:colOff>540360</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>88560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16352,7 +16352,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15679080" y="9050760"/>
-        <a:ext cx="4559040" cy="2780280"/>
+        <a:ext cx="4558680" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16376,9 +16376,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>658080</xdr:colOff>
+      <xdr:colOff>657720</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16387,7 +16387,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16610760" y="180000"/>
-        <a:ext cx="4415400" cy="2782800"/>
+        <a:ext cx="4415040" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16406,9 +16406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>115200</xdr:colOff>
+      <xdr:colOff>114840</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>49320</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16417,7 +16417,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16740360" y="3225240"/>
-        <a:ext cx="4413600" cy="2782800"/>
+        <a:ext cx="4413240" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16436,9 +16436,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>543600</xdr:colOff>
+      <xdr:colOff>543240</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>83160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16447,7 +16447,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16498080" y="6241320"/>
-        <a:ext cx="4413600" cy="2780280"/>
+        <a:ext cx="4413240" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16466,9 +16466,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>351360</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>88560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16477,7 +16477,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16305840" y="9226080"/>
-        <a:ext cx="4413600" cy="2780280"/>
+        <a:ext cx="4413240" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16501,9 +16501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>224640</xdr:colOff>
+      <xdr:colOff>224280</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>10800</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16512,7 +16512,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16848000" y="207360"/>
-        <a:ext cx="4415400" cy="2782800"/>
+        <a:ext cx="4415040" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16531,9 +16531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>23760</xdr:colOff>
+      <xdr:colOff>23400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16542,7 +16542,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15978240" y="3277440"/>
-        <a:ext cx="4413600" cy="2782800"/>
+        <a:ext cx="4413240" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16561,9 +16561,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>18000</xdr:colOff>
+      <xdr:colOff>17640</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16572,7 +16572,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15972480" y="6095880"/>
-        <a:ext cx="4413600" cy="2780280"/>
+        <a:ext cx="4413240" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16591,9 +16591,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>75240</xdr:colOff>
+      <xdr:colOff>74880</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16602,7 +16602,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16029720" y="9158040"/>
-        <a:ext cx="4413600" cy="2780280"/>
+        <a:ext cx="4413240" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16626,9 +16626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>605880</xdr:colOff>
+      <xdr:colOff>605520</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16637,7 +16637,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="17229240" y="207000"/>
-        <a:ext cx="4415400" cy="2782800"/>
+        <a:ext cx="4415040" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16656,9 +16656,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>352800</xdr:colOff>
+      <xdr:colOff>352440</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16667,7 +16667,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15636600" y="3223080"/>
-        <a:ext cx="4413600" cy="2782800"/>
+        <a:ext cx="4413240" cy="2782440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16686,9 +16686,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>451800</xdr:colOff>
+      <xdr:colOff>451440</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
+      <xdr:rowOff>99720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16697,7 +16697,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15735600" y="6082560"/>
-        <a:ext cx="4413600" cy="2780280"/>
+        <a:ext cx="4413240" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16716,9 +16716,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>456480</xdr:colOff>
+      <xdr:colOff>456120</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -16727,7 +16727,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="15740280" y="8996400"/>
-        <a:ext cx="4413600" cy="2780280"/>
+        <a:ext cx="4413240" cy="2779920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16748,7 +16748,7 @@
   <dimension ref="A1:S70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T41" activeCellId="0" sqref="T41"/>
+      <selection pane="topLeft" activeCell="T41" activeCellId="1" sqref="S2:V2 T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18917,8 +18917,8 @@
   </sheetPr>
   <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC24" activeCellId="0" sqref="AC24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC24" activeCellId="1" sqref="S2:V2 AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21089,10 +21089,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S67"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I63" activeCellId="0" sqref="I63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L19" activeCellId="1" sqref="S2:V2 L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21157,6 +21157,18 @@
       <c r="Q2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="S2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
@@ -21210,6 +21222,18 @@
         <f aca="false">(SUM(C3:N3)-O3-P3)/10</f>
         <v>0.17361</v>
       </c>
+      <c r="S3" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
@@ -21263,6 +21287,18 @@
         <f aca="false">(SUM(C4:N4)-O4-P4)/10</f>
         <v>0.6794</v>
       </c>
+      <c r="S4" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
@@ -21316,6 +21352,18 @@
         <f aca="false">(SUM(C5:N5)-O5-P5)/10</f>
         <v>1.51581</v>
       </c>
+      <c r="S5" s="0" t="n">
+        <v>24000</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>13.8</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
@@ -21369,6 +21417,18 @@
         <f aca="false">(SUM(C6:N6)-O6-P6)/10</f>
         <v>2.68145</v>
       </c>
+      <c r="S6" s="0" t="n">
+        <v>32000</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>24.5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
@@ -21422,6 +21482,18 @@
         <f aca="false">(SUM(C7:N7)-O7-P7)/10</f>
         <v>4.23698</v>
       </c>
+      <c r="S7" s="0" t="n">
+        <v>40000</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>39.2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
@@ -21475,6 +21547,18 @@
         <f aca="false">(SUM(C8:N8)-O8-P8)/10</f>
         <v>6.08596</v>
       </c>
+      <c r="S8" s="0" t="n">
+        <v>48000</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>55.3</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <v>55.3</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <v>55.3</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
@@ -21528,6 +21612,18 @@
         <f aca="false">(SUM(C9:N9)-O9-P9)/10</f>
         <v>8.49011</v>
       </c>
+      <c r="S9" s="0" t="n">
+        <v>56000</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>75.4</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>75.4</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>75.4</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -21544,6 +21640,18 @@
       </c>
       <c r="Q14" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21559,6 +21667,18 @@
         <f aca="false">(SUM(C15:N15)-O15-P15)/10</f>
         <v>0</v>
       </c>
+      <c r="S15" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>1.6</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O16" s="0" t="n">
@@ -21573,6 +21693,18 @@
         <f aca="false">(SUM(C16:N16)-O16-P16)/10</f>
         <v>0</v>
       </c>
+      <c r="S16" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>6.1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O17" s="0" t="n">
@@ -21587,6 +21719,18 @@
         <f aca="false">(SUM(C17:N17)-O17-P17)/10</f>
         <v>0</v>
       </c>
+      <c r="S17" s="0" t="n">
+        <v>24000</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>13.8</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O18" s="0" t="n">
@@ -21601,6 +21745,18 @@
         <f aca="false">(SUM(C18:N18)-O18-P18)/10</f>
         <v>0</v>
       </c>
+      <c r="S18" s="0" t="n">
+        <v>32000</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>24.5</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O19" s="0" t="n">
@@ -21615,6 +21771,18 @@
         <f aca="false">(SUM(C19:N19)-O19-P19)/10</f>
         <v>0</v>
       </c>
+      <c r="S19" s="0" t="n">
+        <v>40000</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <v>39.2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O20" s="0" t="n">
@@ -21629,6 +21797,18 @@
         <f aca="false">(SUM(C20:N20)-O20-P20)/10</f>
         <v>0</v>
       </c>
+      <c r="S20" s="0" t="n">
+        <v>48000</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>55.3</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>55.3</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <v>55.3</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O21" s="0" t="n">
@@ -21642,6 +21822,18 @@
       <c r="Q21" s="0" t="n">
         <f aca="false">(SUM(C21:N21)-O21-P21)/10</f>
         <v>0</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <v>56000</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>75.4</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>75.4</v>
+      </c>
+      <c r="V21" s="0" t="n">
+        <v>75.4</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22970,8 +23162,8 @@
   </sheetPr>
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="S2:V2 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23699,8 +23891,8 @@
   </sheetPr>
   <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S47" activeCellId="0" sqref="S47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S47" activeCellId="1" sqref="S2:V2 S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26393,10 +26585,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S69"/>
+  <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26462,6 +26654,18 @@
       <c r="Q2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="S2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
@@ -26939,6 +27143,18 @@
       <c r="Q12" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="S12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
@@ -26992,6 +27208,18 @@
         <f aca="false">(SUM(C13:N13)-O13-P13)/10</f>
         <v>0.149</v>
       </c>
+      <c r="S13" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>1.4</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
@@ -27045,6 +27273,18 @@
         <f aca="false">(SUM(C14:N14)-O14-P14)/10</f>
         <v>0.5976</v>
       </c>
+      <c r="S14" s="0" t="n">
+        <v>15000</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>5.4</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
@@ -27098,6 +27338,18 @@
         <f aca="false">(SUM(C15:N15)-O15-P15)/10</f>
         <v>1.3467</v>
       </c>
+      <c r="S15" s="0" t="n">
+        <v>22500</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>12.1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
@@ -27151,6 +27403,18 @@
         <f aca="false">(SUM(C16:N16)-O16-P16)/10</f>
         <v>2.4001</v>
       </c>
+      <c r="S16" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>21.5</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
@@ -27204,6 +27468,18 @@
         <f aca="false">(SUM(C17:N17)-O17-P17)/10</f>
         <v>3.744</v>
       </c>
+      <c r="S17" s="0" t="n">
+        <v>37500</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
@@ -27257,6 +27533,18 @@
         <f aca="false">(SUM(C18:N18)-O18-P18)/10</f>
         <v>5.4</v>
       </c>
+      <c r="S18" s="0" t="n">
+        <v>45000</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>48.5</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
@@ -27310,6 +27598,18 @@
         <f aca="false">(SUM(C19:N19)-O19-P19)/10</f>
         <v>7.3547</v>
       </c>
+      <c r="S19" s="0" t="n">
+        <v>52500</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>66.8</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>66.8</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <v>66.8</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
@@ -27362,6 +27662,18 @@
       <c r="Q20" s="0" t="n">
         <f aca="false">(SUM(C20:N20)-O20-P20)/10</f>
         <v>9.6</v>
+      </c>
+      <c r="S20" s="0" t="n">
+        <v>60000</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>86.7</v>
+      </c>
+      <c r="U20" s="0" t="n">
+        <v>86.7</v>
+      </c>
+      <c r="V20" s="0" t="n">
+        <v>86.7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28855,7 +29167,7 @@
   <dimension ref="A1:V69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
+      <selection pane="topLeft" activeCell="S11" activeCellId="1" sqref="S2:V2 S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29423,6 +29735,18 @@
       <c r="Q12" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="S12" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
@@ -29476,6 +29800,18 @@
         <f aca="false">(SUM(C13:N13)-O13-P13)/10</f>
         <v>0.036</v>
       </c>
+      <c r="S13" s="0" t="n">
+        <v>15000</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>5.4</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
@@ -29529,6 +29865,18 @@
         <f aca="false">(SUM(C14:N14)-O14-P14)/10</f>
         <v>0.145</v>
       </c>
+      <c r="S14" s="0" t="n">
+        <v>22500</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>12.1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
@@ -29582,6 +29930,18 @@
         <f aca="false">(SUM(C15:N15)-O15-P15)/10</f>
         <v>0.3256</v>
       </c>
+      <c r="S15" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>21.6</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>21.6</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
@@ -29635,6 +29995,18 @@
         <f aca="false">(SUM(C16:N16)-O16-P16)/10</f>
         <v>0.5784</v>
       </c>
+      <c r="S16" s="0" t="n">
+        <v>37500</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
@@ -29688,6 +30060,18 @@
         <f aca="false">(SUM(C17:N17)-O17-P17)/10</f>
         <v>0.9085</v>
       </c>
+      <c r="S17" s="0" t="n">
+        <v>45000</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>48.5</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
@@ -29741,6 +30125,18 @@
         <f aca="false">(SUM(C18:N18)-O18-P18)/10</f>
         <v>1.3116</v>
       </c>
+      <c r="S18" s="0" t="n">
+        <v>52500</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>66.9</v>
+      </c>
+      <c r="U18" s="0" t="n">
+        <v>66.9</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <v>66.9</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
@@ -29793,6 +30189,18 @@
       <c r="Q19" s="0" t="n">
         <f aca="false">(SUM(C19:N19)-O19-P19)/10</f>
         <v>1.7768</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <v>60000</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>86.7</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <v>86.7</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <v>86.7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31307,7 +31715,7 @@
   <dimension ref="A1:V67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S19" activeCellId="0" sqref="S19"/>
+      <selection pane="topLeft" activeCell="S19" activeCellId="1" sqref="S2:V2 S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33735,8 +34143,8 @@
   </sheetPr>
   <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S47" activeCellId="0" sqref="S47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S47" activeCellId="1" sqref="S2:V2 S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>